<commit_message>
back to renesas from mcu
</commit_message>
<xml_diff>
--- a/TDigikey_upload.xlsx
+++ b/TDigikey_upload.xlsx
@@ -430,3500 +430,3500 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>UPD70F3505AGCA1-UEU-AX</t>
+          <t>DA9063L-XXHO1-AT</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>UPD703209GK(A2)-9EU-A</t>
+          <t>DA9063L-XXHO2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>R5F564MGCDFB#31</t>
+          <t>DA9063L-XXHO2-AT</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>R7F7016104AFP-C</t>
+          <t>DA9063-XXHK1-A</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>R5F11ZBADFP#50</t>
+          <t>DA9063-XXHO1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>R5F571MFCGFB#V0</t>
+          <t>DA9063-XXHO1-A</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>R5F51101AGNE#U0</t>
+          <t>DA9063-XXHO1-AT</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>R5F562GAADFP#V3</t>
+          <t>DA9063-XXHO2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>R5F56519FDFP#30</t>
+          <t>DA9063-XXHO2-A</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>R7F100GMK2DFB#HA0</t>
+          <t>DA9063-XXHO2-AT</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>R5F572TFCGFB#30</t>
+          <t>DA9066</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>R5F10DGELFB#H2</t>
+          <t>DA9066-03</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>R5F563NACDFB#V0</t>
+          <t>DA9066-EVAL</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UPD70F3368GJ(A)-UEN-A</t>
+          <t>DA9068</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>R7FS5D97E3A01CFB#AA0</t>
+          <t>DA9068-ABUT2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>R5F52315CDND#U0</t>
+          <t>DA9070-00V32</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>R7FA4E10B2CNE#AA0</t>
+          <t>DA9070-00XX</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>R5F101EGANA#00</t>
+          <t>DA9070-08V32</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>R5F56318CDLK#U0</t>
+          <t>DA9070-08V36</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>R5F56604AGFL#30</t>
+          <t>DA9070-09V32</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>R5F10EGEGFB#X0</t>
+          <t>DA9070-09V36</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>R5F52107CDFN#30</t>
+          <t>DA9070-0EV36</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>R5F101GHAFB#V0</t>
+          <t>DA9070-FG-EVAL3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>R7F102G7E2DNP#HA0</t>
+          <t>DA9070-ODV32</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>R7F100GPG3CFB#BA0</t>
+          <t>DA9070-XXXX</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>R5F1017DDNA#W0</t>
+          <t>DA9072-80V32</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>R5F52305ADND#00</t>
+          <t>DA9072-82V32</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>R5F100LGAFB#V0</t>
+          <t>DA9073-00XX</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>R5F563NECDLC#U0</t>
+          <t>DA9073-61V32</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>R5F104MJGFA#50</t>
+          <t>DA9073-62V32</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>R5F104LJAFB#X0</t>
+          <t>DA9073-62V36</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>R7F100GPL2DFB#HA0</t>
+          <t>DA9073-6BV32</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>R5F10DPGCJFB#56G</t>
+          <t>DA9073-XXXX</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>R7F100GFG2DFP#HA0</t>
+          <t>DA9080</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>R5F11W68ASM#50</t>
+          <t>DA9080-XXFC2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R5F565N4BGFB#10</t>
+          <t>DA9083-XXUUA2</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>R5F5651CDGFM#10</t>
+          <t>DA9083-XXUUA6</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>R5F564MJGDLJ#21</t>
+          <t>DA9121-A0V72</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>R5F10AGECKFB#35</t>
+          <t>DA9121-A2V72</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>R5F566NDHGFC#V0</t>
+          <t>DA9121-B0V72</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>R7F100GFL2DFP#BA0</t>
+          <t>DA9122-E1V72</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>R5F10PADYSP#G5</t>
+          <t>DA9122-E1V76</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>R5F101JKAFA#X0</t>
+          <t>DA9130-A</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>R5F5651EDDFB#10</t>
+          <t>DA9130-XXRT1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R5F104LEAFP#10</t>
+          <t>DA9130-XXRT1-A</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R5F563NDDDFC#V0</t>
+          <t>DA9130-XXRT2</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>R5F10366ASP#55</t>
+          <t>DA9130-XXRT2-A</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>R5F572NDHGFC#V0</t>
+          <t>DA9130-XXRT2-AT</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>R7F100GMH2DFA#BA0</t>
+          <t>DA9131-A</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>RL78/L1C</t>
+          <t>DA9131-XXRT1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>R5F100FADFP#30</t>
+          <t>DA9131-XXRT1-AT</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>R5F101EHDNA#U0</t>
+          <t>DA9131-XXRT2</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>R5F104LHAFA#V0</t>
+          <t>DA9131-XXRT2-A</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>UPD70F3622M2GCA1-UEU-AX</t>
+          <t>DA9131-XXRT2-AT</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>R5F100LFDFA#X0</t>
+          <t>DA9132-A</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>R5F101GHDFB#30</t>
+          <t>DA9132-XXRT1</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>R5F571MGDGFB#V0</t>
+          <t>DA9132-XXRT1-AT</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>R5F5631ACDFC#V0</t>
+          <t>DA9132-XXRT2</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>R5F109GCKFB#X0G</t>
+          <t>DA9132-XXRT2-A</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>R5F104GFANA#20</t>
+          <t>DA9155M-02U72</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>R9A07G043F01GBG#AC0</t>
+          <t>DA9155M-EVAL1</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>R5F566TAAGFF#30</t>
+          <t>DA9155M-XXU72</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>R5F51117AGFM#1A</t>
+          <t>DA9168</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>R5F56719DDFM#10</t>
+          <t>DA9168-XXU72</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>R5F111PFAFB#10</t>
+          <t>DA9210-A</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>R5F572TFAGFP#10</t>
+          <t>DA9211</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>R5F101GKANA#20</t>
+          <t>DA9211-00UU6</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>R5F572TKCDFB#30</t>
+          <t>DA9211-50UU2</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>R7FA6T2AD3CFL#AA1</t>
+          <t>DA9212-00UU2</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>R5F10RBCGFP#50</t>
+          <t>DA9212-00UU6</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>R5F52305AGNE#00</t>
+          <t>DA9212-50UU2</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>R5F104GCGNA#20</t>
+          <t>DA9212-AKUU2</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>R5F51118ADNE#0A</t>
+          <t>DA9213-00UP2</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>R5F104JFAFA#30</t>
+          <t>DA9213-00UP6</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>R5F10PLHYFB#H5</t>
+          <t>DA9213-50UP2</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>R5F52107CGFN#30</t>
+          <t>DA9213-A-EVAL1</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>R5F56317DGFP#V0</t>
+          <t>DA9213-C1FS2-A</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>R5F51113AGFK#3A</t>
+          <t>DA9213-C1FS2BB-A</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>R7S921040VCBG#AC0</t>
+          <t>DA9213-EVAL1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>UPD70F3354GJ(A)-GAE-AX</t>
+          <t>DA9213-XXFS1-A</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>R5F563NFDGFC#V0</t>
+          <t>DA9213-XXFSC</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>R5F52315AGND#00</t>
+          <t>DA9213-XXUP2</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>R5F5631PCDFM#V0</t>
+          <t>DA9214-00FS1-A</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>R5F51406AGFK#10</t>
+          <t>DA9214-00FS2-A</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>R5F104GDGNA#20</t>
+          <t>DA9214-00UP2</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>R5F104MGGFB#V0</t>
+          <t>DA9214-50UP2</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>R5F566TEEDFM#10</t>
+          <t>DA9214-A</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>R5F10DPKJFB#H2G</t>
+          <t>DA9214-C3FS2-A</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>R7F7010494AFP</t>
+          <t>DA9214-XXFSC</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>R5F51303ADNE#20</t>
+          <t>DA9214-XXFSC-AT</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>R5F101MFAFA#10</t>
+          <t>DA9214-XXUP2</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>R5F100GFANA#W0</t>
+          <t>DA9215-00UP2</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>R7FA6M5BG2CBG#AC0</t>
+          <t>DA9215-00UP6</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>R5F565N4BDFP#10</t>
+          <t>DA9215-50UP2</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>R5F1026AASP#X0</t>
+          <t>DA9215-XXFS1-AT</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>R5F56609DGFP#30</t>
+          <t>DA9215-XXFSC</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>R5F10RLCGFB#50</t>
+          <t>DA9215-XXFSC-A</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>UPD70F3621M1GCA1-UEU-AX</t>
+          <t>DA9215-XXUP2</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>R5F100PKAFA#X0</t>
+          <t>DA9215-XXUP6</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>R5F101GKANA#U0</t>
+          <t>DA9217-20V72</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>R5F5631BCDFB#V0</t>
+          <t>DA9217-20V76</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>R5F56517EGFP#30</t>
+          <t>DA9217-EVAL1</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>R5F104GLGNA#40</t>
+          <t>DA9217-XXV72</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>R5F100AGDSP#X0</t>
+          <t>DA9217-XXV76</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>R5F100LJGFA#30</t>
+          <t>DA9220-70V72</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>R5F102A7GSP#X0</t>
+          <t>DA9220-70V76</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>R5F104LHGFA#30</t>
+          <t>DA9220-71V72</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>R5F12017GSP#30</t>
+          <t>DA9220-71V76</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>R7FA2E1A53CNE#HA0</t>
+          <t>DA9220-EVAL1</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>R5F566TEAGFM#10</t>
+          <t>DA9220-XXV72</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>R5F562N7BDBG#U0</t>
+          <t>DA9224-A</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>R5F1076CMSP#X0</t>
+          <t>DA9230-00VZ2</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>UPD70F3210YGC(A2)-8BT-A</t>
+          <t>DA9230-07VZ2</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>R7F7010244AFP</t>
+          <t>DA9230-09VZ2</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>R5F102A9DSP#30</t>
+          <t>DA9230-0AVZ2</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>R5F563TBADFB#V0</t>
+          <t>DA9230-XXVZ2</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>R5F101FDAFP#10</t>
+          <t>DA9231-00VZ2</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>R5F564MFGDFP#V1</t>
+          <t>DA9231-0BVZ2</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>R7F100GEG2DNP#HA0</t>
+          <t>DA9231-0CVZ2</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>R7FA2E1A92DFK#HA0</t>
+          <t>DA9231-0DVZ2</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>R5F10BMGYFB#X5</t>
+          <t>DA9231-XXVZ2</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>R5F140GLAFB#30</t>
+          <t>DA9232-81VZ2</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>R5F101GEANA#40</t>
+          <t>DA9232-82VZ2</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>R5F101ADASP#50</t>
+          <t>DA9232-XXVZ2</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>R5F11BCCALA#U0</t>
+          <t>DA9233-A1VZ2</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>R5F562T6EDFF#V1</t>
+          <t>DA9233-XXVZ2</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>R5F1027ADNA#W0</t>
+          <t>DA9313-02VK2</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>R5F563T5EGFL#V0</t>
+          <t>DA9313-02VK6</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>R7F100GFH3CFP#BA0</t>
+          <t>DA9313-03VK2</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>R7FS1JA783A01CFM#BA0</t>
+          <t>DA9313-03VK6</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>R5F51118ADFL#3A</t>
+          <t>DA9313-04VK2</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>UPD70F3210GC(A1)-8BT-A</t>
+          <t>DA9313-04VK6</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>R5F104BEANA#00</t>
+          <t>DA9313-08VK2</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>R5F571MJCDFC#30</t>
+          <t>DA9313-10VK2</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>R5F10Y44ASP#10</t>
+          <t>DA9313-24VK2</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>R5F100GGGFB#50</t>
+          <t>DA9318L</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>R5F10BLGKFB#H5</t>
+          <t>DA9318L-06UF2</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>R5F10PGFCLFB#55</t>
+          <t>DA9318M-06UF2</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>R5F100LCGFA#30</t>
+          <t>DG403DVZ</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>R5F100PKDFB#10</t>
+          <t>DG403DY</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>R9A07G063U02GBG#BC0</t>
+          <t>DG403DYZ</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>R5F100MLAFA#10</t>
+          <t>DG403EJ</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>R5F566TFADFP#30</t>
+          <t>DG403EY</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>R5F100FEDFP#50</t>
+          <t>DG406DJ</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>R7F701205EAFP</t>
+          <t>DG406DJZ</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>R5F10RLCGNB#U0</t>
+          <t>DG406DY</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>R5F562GADDFH#V3</t>
+          <t>DG406DYZ</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>R7FA2L1A93CFN#AA0</t>
+          <t>DG406DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>R7FA6M4AF2CBM#BC0</t>
+          <t>DG406EY</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>R5F1007CDNA#W0</t>
+          <t>DG407DJ</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>R5F10266DSP#55</t>
+          <t>DG407DJZ</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>R5F10AMECLFB#35</t>
+          <t>DG407DYZ</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>R5F56719HGFP#10</t>
+          <t>DG407DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>R5F100GDAFB#50</t>
+          <t>DG407EJ</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>R5F104LDDFB#30</t>
+          <t>DG408DJ</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>R5F104LHAFB#50</t>
+          <t>DG408DJZ</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>R5F51111AGFK#1A</t>
+          <t>DG408DVZ</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>R7F100GAJ2DSP#HA0</t>
+          <t>DG408DYZ</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>R5F51116AGFL#1A</t>
+          <t>DG408DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>R5F104GKGNA#20</t>
+          <t>DG409DJ</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>R5F100MJDFA#X0</t>
+          <t>DG409DJZ</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>R5F103A7ASP#50</t>
+          <t>DG409DVZ</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>R5F51403AGNE#30</t>
+          <t>DG409DVZ-T</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>R5F56604CDFP#10</t>
+          <t>DG409DYZ</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>R5F104GJANA#20</t>
+          <t>DG409DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>R7F100GGN2DFB#AA0</t>
+          <t>DG409EJ</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>R5F101FEAFP#30</t>
+          <t>DG411DVZ-T</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>R5F565N9BGFB#10</t>
+          <t>DG411DYZ</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>R5F56719HGBP#20</t>
+          <t>DG411DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>R5F56604EGFB#10</t>
+          <t>DG412DVZ-T</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>R5F56604BGFP#10</t>
+          <t>DG412DYZ</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>R5F104BAGNA#W0</t>
+          <t>DG412DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>R5F571MFHGFB#V0</t>
+          <t>DG413DJZ</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>UPD70F3555AM1GMA2-GBK-AX</t>
+          <t>DG413DYZ</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>R7F701278EAFP#AC6</t>
+          <t>DG413DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>R5F100EDGNA#20</t>
+          <t>DG441AK/883</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>R5F51104AGFL#10</t>
+          <t>DG441DJZ</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>R5F564MFHDFC#11</t>
+          <t>DG441DVZ</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>R5F101BDANA#40</t>
+          <t>DG441DVZ-T</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>R5F101CFALA#W0</t>
+          <t>DG441DYZ</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>R5F10PMHCLFB#55</t>
+          <t>DG441DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>R5F56514EGFB#10</t>
+          <t>DG441EY</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>R5F10AAELSP#W5</t>
+          <t>DG442DJZ</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>R5F101GCAFB#30</t>
+          <t>DG442DVZ</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>R5F100JLAFA#V0</t>
+          <t>DG442DVZ-T</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>R5F5631FDDFP#V0</t>
+          <t>DG442DYZ</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>R5F571MJCDFP#10</t>
+          <t>DG442DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>R5F104LEALA#W0</t>
+          <t>DG444DVZ-T</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>R5F564MJHDFP#V1</t>
+          <t>DG444DY</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>R5F565NEDDFC#30</t>
+          <t>DG444DYZ</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>R9A07G043U16GBG#BC0</t>
+          <t>DG444DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>R5F5631DDDFP#V0</t>
+          <t>DG445DJ</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>R5F51111AGNF#UA</t>
+          <t>DG445DVZ</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>R5F571MGCGFB#V0</t>
+          <t>DG445DVZ-T</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>R5F10BBCKNA#G5</t>
+          <t>DG445DY</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>R7F100GLH2DFA#HA0</t>
+          <t>DG445DYZ</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>R5F56316CDBG#U0</t>
+          <t>DG445DYZ-T</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>R5F10CGDJFB#X6G</t>
+          <t>EL4340IU</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>R5F10WLGAFA#50</t>
+          <t>EL4340IU-T13</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>R5F51406AGFM#30</t>
+          <t>EL4340IU-T7</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>R5F562N8BDFP#V0</t>
+          <t>EL4340IUZ</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>R7FA2E1A92DFJ#AA0</t>
+          <t>EL4340IUZ-T13</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>R5F52316CGNE#20</t>
+          <t>EL4340IUZ-T7</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>R5F10BGEKFB#X5</t>
+          <t>EL4543IL</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>R8A77440HA02BG#UA</t>
+          <t>EL4543IL-T13</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>R5F104EFANA#W0</t>
+          <t>EL4543ILZ-T7</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>R5F104MGGFA#30</t>
+          <t>EL4543IU</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>R5F572NNHGFB#30</t>
+          <t>EL4543IUZ-T7</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>R7FA6M2AD3CFB#AA0</t>
+          <t>EL5106IS</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>R5F101PKAFA#V0</t>
+          <t>EL5106ISZ</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>R5F571MLGDFB#30</t>
+          <t>EL5106ISZ-T13</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>R5F572MNHDFP#10</t>
+          <t>EL5106IWZ-T7</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>R5F113PHCKFB#15</t>
+          <t>EL5106IWZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>R5F10EGCANA#00</t>
+          <t>EL5111IWTZ-T7</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>R9A06G032VGBG#AC1</t>
+          <t>EL5111IWTZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>R5F10PGGYFB#H5</t>
+          <t>EL5111IYEZ</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>R5F12047ASP#30</t>
+          <t>EL5111IYEZ-T13</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>R5F100MFDFA#50</t>
+          <t>EL5111IYEZ-T7</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>R5F104LGGFB#50</t>
+          <t>EL5111TIWTZ-T7</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>R5F562T6DDFM#13</t>
+          <t>EL5111TIWTZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>R5F104GJAFB#10</t>
+          <t>EL5160ISZ</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>R5F11BGCAFB#50</t>
+          <t>EL5160ISZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>R5F523E6SDFL#10</t>
+          <t>EL5160IWZ-T7</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>R7S921051VCBG#AC0</t>
+          <t>EL5160IWZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>R7FA2E1A52DFL#BA0</t>
+          <t>EL5161IC-T7A</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>R5F56517BDLK#20</t>
+          <t>EL5161IWZ-T7</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>UPD70F3613M1GBA1-GAH-AX</t>
+          <t>EL5161IWZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>R5F10PBEYNA#G5</t>
+          <t>EL5166ISZ</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>R5F51303ADFN#30</t>
+          <t>EL5166ISZ-T7</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>R5F565NCDGFP#30</t>
+          <t>EL5166IWZ-T7</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>R5F104LFGLA#W0</t>
+          <t>EL5166IWZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>R7F100GFG2DFP#BA0</t>
+          <t>EL5172IS</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>R5F565NCDDLC#20</t>
+          <t>EL5172ISZ</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>R5F100PGGFA#30</t>
+          <t>EL5172ISZ-T7</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>R7FA2E1A72DFK#BA0</t>
+          <t>EL5172ISZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>R5F10CGBLFB#H2G</t>
+          <t>EL5172IY-T7</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>R5F104LFDFP#X0</t>
+          <t>EL5172IYZ-T13</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>R5F104MHDFA#50</t>
+          <t>EL5172IYZ-T7</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>R7F7010074AFP</t>
+          <t>EL5220CY</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>R5F10ABCYNA#G5</t>
+          <t>EL5220CY-T13</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>R5F1176AGSP#50</t>
+          <t>EL5220CY-T7</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>UPD70F3617M2GKA1-GAK-AX</t>
+          <t>EL5220CYZ</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>UPD70F3478AGJA-GAE-G</t>
+          <t>EL5220CYZ-T13</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>R5F117GAGFB#30</t>
+          <t>EL5220CYZ-T7</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>R5F104GJAFB#30</t>
+          <t>EL5220TILZ-T13</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>R5F100GEGNA#00</t>
+          <t>EL5220TIYZ</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>R5F104FAAFP#30</t>
+          <t>EL5220TIYZ-T13</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>R5F10WLDAFB#30</t>
+          <t>EL5220TIYZ-T7</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>R5F109LCKFB#H0</t>
+          <t>EL5262IY-T7</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>R5F104LJALA#U0</t>
+          <t>EL5262IYZ</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>R5F56609DDFP#10</t>
+          <t>EL5262IYZ-T13</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>R7FA6T2BD3CFM#AA1</t>
+          <t>EL5262IYZ-T7</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>R5F100LHGBG#U0</t>
+          <t>EL5263IS-T13</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>UPD70F3503M2GCA2-UEU-AX</t>
+          <t>EL5263IS-T7</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>R7F100GGF3CNP#HA0</t>
+          <t>EL5263ISZ</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>R7FA6E2B92CBB#BC0</t>
+          <t>EL5263ISZ-T13</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>R5F563TEBDFH#V0</t>
+          <t>EL5263ISZ-T7</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>R5F56307DDFP#V0</t>
+          <t>EL5263IYZ</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>R5F10PGJLNA#U5</t>
+          <t>EL5263IYZ-T13</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>R5F1007DANA#U0</t>
+          <t>EL5306IS</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>R5F56719HDLJ#20</t>
+          <t>EL5306IS-T13</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>R5F100MFAFB#X0</t>
+          <t>EL5306ISZ-T7</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>R5F51135AGFM#1A</t>
+          <t>EL5306IU-T13</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>R7F7010103AFP</t>
+          <t>EL5306IUZ</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>R5F10PMFLFB#X5</t>
+          <t>EL5306IUZ-T13</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>R5F104BGDFP#50</t>
+          <t>EL5306IUZ-T7</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>R5F565N4ADFB#30</t>
+          <t>EL5375IU</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>R5F10RGCGFB#30</t>
+          <t>EL5375IU-T13</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>R5F51403ADFJ#30</t>
+          <t>EL5375IU-T7</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>R5F5671CHGBP#20</t>
+          <t>EL5375IUZ-T7</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>R5F56609ADFP#10</t>
+          <t>EL5378IU</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>UPD70F3752GC(R)-UEU-AX</t>
+          <t>EL5378IU-T7</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>R5F5631FDGFP#V0</t>
+          <t>EL5378IUZ</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>R5F100LJAFB#V0</t>
+          <t>EL5378IUZ-T13</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>R5F104LEAFA#30</t>
+          <t>EL5378IUZ-T7</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>R9A07G084M08GBA#AC0</t>
+          <t>EL5420CR</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>R5F10PLGCLFB#55</t>
+          <t>EL5420CR-T13</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>R5F104GCGFB#50</t>
+          <t>EL5420CR-T7</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>R5F51118ADLF#UA</t>
+          <t>EL5420CRZ</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>R5F10CGBCJFB#12</t>
+          <t>EL5420CRZ-T13</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>R5F56318DDFP#V0</t>
+          <t>EL5420CRZ-T7</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>R5F100BDGNA#W0</t>
+          <t>EL5420CRZ-T7A</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>R5F101PHDFB#V0</t>
+          <t>EL5420CSZ</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>R5F5671EHDFB#10</t>
+          <t>EL5420TILZ</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>R5F104PLAFA#V0</t>
+          <t>EL5420TIRZ</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>R5F10PGECLFB#15</t>
+          <t>EL5420TISZ-T13</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>R5F11MPFAFB#50</t>
+          <t>EL5462IS</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>R5F10CGBCJFB#12G</t>
+          <t>EL5462IS-T13</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>R5F109LEJFB#H0G</t>
+          <t>EL5462IS-T7</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>R5F521A8BGFN#30</t>
+          <t>EL5462ISZ</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>R5F101GCDNA#W0</t>
+          <t>EL5462ISZ-T13</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>R5F562N7ADBG#00</t>
+          <t>EL5462ISZ-T7</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>R7F701388EAFP</t>
+          <t>EL7104CN</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>R5F100EEDNA#W0</t>
+          <t>EL7104CNZ</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>R5F10TPJCLFB#12G</t>
+          <t>EL7104CS</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>R5F101LHABG#W0</t>
+          <t>EL7104CSZ</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>R7FA2L1AB3CFM#AA0</t>
+          <t>EL7104CSZ-T13</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>R5F52316CDFM#30</t>
+          <t>EL7104CSZ-T7</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>R5F104FADFP#30</t>
+          <t>EL7202CN</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>R5F10EGAAFB#X0</t>
+          <t>EL7202CS</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>R5F563TEADFP#V0</t>
+          <t>EL7202CS-T7</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>R5F566TKGDFP#10</t>
+          <t>EL7202CSZ</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>R5F571MLCGFB#V0</t>
+          <t>EL7202CSZ-T7</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>R5F51103AGNF#20</t>
+          <t>EL7212CN</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>R5F109GDCKFB#10</t>
+          <t>EL7212CNZ</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>R5F10RLAAFA#10</t>
+          <t>EL7212CS</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>R5F51306BGFL#30</t>
+          <t>EL7212CSZ</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>R5F109GECJFB#10G</t>
+          <t>EL7212CSZ-T13</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>R5F56609CDFN#30</t>
+          <t>EL7212CSZ-T7</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>R7F100GJN3CFA#BA0</t>
+          <t>EL7222CS</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>R5F566TAAGFN#10</t>
+          <t>EL7222CSE9044-T7</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>RZ/G1M</t>
+          <t>EL7222CS-T7</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>R5F101LDABG#U0</t>
+          <t>EL7222CSZ</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>R5F104EDANA#W0</t>
+          <t>EL7222CSZ-T13</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>R5F100EDGNA#U0</t>
+          <t>EL7222CSZ-T7</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>R5F10DPGLFB#H2G</t>
+          <t>EL7232CNZ</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>R5F5111JADFM#3A</t>
+          <t>EL7232CS</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>R5F52317BGFM#10</t>
+          <t>EL7232CSZ</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>R5F101GLANA#W0</t>
+          <t>EL7232CSZ-T13</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>R5F5631MCDFM#V0</t>
+          <t>EL7242CS</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>R5F523E5AGFL#10</t>
+          <t>EL7242CS-T13</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>R5F104LHDFB#50</t>
+          <t>EL7242CS-T7</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>R5F10PGDLNA#G5</t>
+          <t>EL7242CSZ-T13</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>R5F562T7BDFM#V3</t>
+          <t>EL7242CSZ-T7</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>R5F100GADFB#X0</t>
+          <t>EL7252CN</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>R5F10AMGKFB#X5</t>
+          <t>EL7252CSZ</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>R5F563TBADFH#V1</t>
+          <t>EL7252CSZ-T13</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>R5F5651EDDBG#20</t>
+          <t>EL7252CSZ-T7</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>R5F572MNDDFB#10</t>
+          <t>EL7530IY</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>R7F701426EABG</t>
+          <t>EL7530IY-T13</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>RZ/G2N</t>
+          <t>EL7530IY-T7</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>R7F100GBF3CFP#AA0</t>
+          <t>EL7530IYZ-T13</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>R5F571MJDDBG#20</t>
+          <t>EL7530IYZ-T13S2695</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>R5F101LDAFB#50</t>
+          <t>EL7530IYZ-T7</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>R5F10367ASP#X5</t>
+          <t>EL7531EVAL1Z</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>R5F10PLECKFB#15</t>
+          <t>EL7531IY</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>R7FA2E1A53CFL#AA0</t>
+          <t>EL7531IY-T7</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>R5F56216BDFB#10</t>
+          <t>EL7531IYZ</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>UPD70F4002AM1GCA2-UEU-AX</t>
+          <t>EL7531IYZ-T13</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>R5F104EDANA#40</t>
+          <t>EL7531IYZ-T7</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>R5F5210BBDFP#10</t>
+          <t>EL7536EVAL1</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>R5F56609AGFM#30</t>
+          <t>EL7536IY</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>R5F565NEHGLC#20</t>
+          <t>EL7536IY-T7</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>R7FA6M4AE3CFB#AA0</t>
+          <t>EL7536IYZ</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>R5F1054AANA#00</t>
+          <t>EL7536IYZ-T</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>R5F565N7FDLJ#20</t>
+          <t>EL7536IYZ-T13</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>R5F1006DDSP#X0</t>
+          <t>EL7536IYZ-T7</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>R5F563T6EDFM#10</t>
+          <t>EL8201IS</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>R5F10EGAGNA#U0</t>
+          <t>EL8201IS-T13</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>R5F56517FGLK#20</t>
+          <t>EL8201IS-T7</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>R5F5631BDDFP#10</t>
+          <t>EL8201ISZ</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>UPD70F3380M2GJA2-GAE-AX</t>
+          <t>EL8201ISZ-T13</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>R7F100GGH2DFB#AA0</t>
+          <t>EL8201ISZ-T7</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>R5F100JGGFA#50</t>
+          <t>EXP8602-DNT</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>R5F10367DSP#V0</t>
+          <t>F0109</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>R7F102GEE2DNP#HA0</t>
+          <t>F0109EVB</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>R5F52108CGFM#30</t>
+          <t>F0109NBTI</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>R7FA2E2A72DNJ#AA1</t>
+          <t>F0109NBTI8</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>R5F101BFANA#00</t>
+          <t>F0110EVB</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>R5F101SHAFB#X0</t>
+          <t>F0110NBTI</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>R5F104LGDFA#30</t>
+          <t>F0110NBTI8</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>R5F10BADKSP#G5</t>
+          <t>F0111EVB</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>R7F7016863AFP-C</t>
+          <t>F0111EVB-2P6</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>R7F100GMN3CFB#BA0</t>
+          <t>F0111NBTI</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>R5F109GDCJFB#50G</t>
+          <t>F0111NBTI8</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>R7F100GGG3CNP#HA0</t>
+          <t>F0424EVBK</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>R5F101SKAFB#30</t>
+          <t>F0424NTGK</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>R5F101EEDNA#W0</t>
+          <t>F0424NTGK8</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>R5F51105AGFL#10</t>
+          <t>F0440EVBI</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>R5F101FGDFP#30</t>
+          <t>F0440NBGI</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>UPD703015AYF1-EA6-A</t>
+          <t>F0440NBGI/W</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>R5F10RBAAFP#V0</t>
+          <t>F0440NBGI8</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>R5F566TKGDFP#30</t>
+          <t>F0443EVB</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>R5F109LECKFB#50</t>
+          <t>F0443LGRI8</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>R7FA2E1A73CFK#AA0</t>
+          <t>F0448EVB</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>R5F10EGDANA#W0</t>
+          <t>F0448EVS</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>R5F100LKDFA#10</t>
+          <t>F0448NBGK</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>R5F10RG8AFB#X0</t>
+          <t>F0448NBGK8</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>R5F5651CDDFC#30</t>
+          <t>F0452BEVB</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>R7F7015863AFP-C</t>
+          <t>F0452BLEGK</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>R5F52106BDFL#30</t>
+          <t>F0452BLEGK8</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>R5F563NBDGFP#V0</t>
+          <t>F0452CEVB</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>R5F1018EALA#U0</t>
+          <t>F0452CLFGK</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>R5F101EHANA#U0</t>
+          <t>F0452CLFGK8</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>R5F104LJGFB#10</t>
+          <t>F0453B</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>R5F564MGDDFB#31</t>
+          <t>F0453BEVB</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>R7F102GAE3CSP#HA0</t>
+          <t>F0453BLEGK</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>R5F5631ECDBG#U0</t>
+          <t>F0453BLEGK8</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>R7F100GGH3CFB#AA0</t>
+          <t>F0453CEVB</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>R5F101PHAFB#50</t>
+          <t>F0453CLEGK</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>R5F10378ANA#45</t>
+          <t>F0453CLFGK</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>R5F100AEASP#V0</t>
+          <t>F0453CLFGK8</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>R5F101JEDFA#30</t>
+          <t>F0480EVB-HBI</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>R5F104LDDFP#30</t>
+          <t>F0480EVBI</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>R5F10PGJYFB#H5</t>
+          <t>F0480EVB-LBI</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>R5F100BGGNA#20</t>
+          <t>F0480EVB-MBI</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>R5F571MGDDLK#20</t>
+          <t>F0480EVS-HBI</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>R5F565N4ADLJ#20</t>
+          <t>F0480EVS-LBI</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>RH850/E1M-S2</t>
+          <t>F0480EVS-MBI</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>R5F566TEADFF#30</t>
+          <t>F0480NBGI</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>R5F10DGECLFB#56G</t>
+          <t>F0502EVBI</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>R5F101GHDFB#50</t>
+          <t>F0502NLGI</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>R5F566TFCGFB#30</t>
+          <t>F0502NLGI8</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>R7FA2E1A72DFM#AA0</t>
+          <t>F0552EVBI</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>R5F10RLCAFA#V0</t>
+          <t>F0552NLGI8</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>R5F563NECDBG#U0</t>
+          <t>F0562EVBI</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>R5F572NDDGBD#20</t>
+          <t>F0562NLGI</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>UPD70F3214GC-8EU-A</t>
+          <t>F0562NLGI8</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>R5F104GHGNA#40</t>
+          <t>F1100</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>R5F51403ADNE#10</t>
+          <t>F1100ANBGI</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>R5F11W67DSM#30</t>
+          <t>F1100BNBGI</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>R5F10PLJYFB#U5</t>
+          <t>F1100BNBGI8</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>R5F564MFHDBG#21</t>
+          <t>F1100NBGI</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>R5F56609CGFM#10</t>
+          <t>F1100NBGI8</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>R5F571MJDDFC#V0</t>
+          <t>F1102</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>R5F10268GSP#55</t>
+          <t>F1102EVBI</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>R7FA6T2BD3CNE#AA1</t>
+          <t>F1102NBGI8</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>R5F100LDAFA#10</t>
+          <t>F1102NBGI8(4)</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>R5F564MJHDFB#31</t>
+          <t>F1129EVB</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>R5F109LEJFB#H0</t>
+          <t>F1129HBNELI</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>R5F100AAGSP#30</t>
+          <t>F1129HBNELI8</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>R5F100LDDFB#V0</t>
+          <t>F1129LBNELI8</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>R5F10BMGLFB#H5</t>
+          <t>F1129MB</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>R5F11ZBAAFP#10</t>
+          <t>F1129MBEVB</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>R5F11TLGDFB#35</t>
+          <t>F1129MBNELI</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>R5F10RLCAFB#30</t>
+          <t>F1129MBNELI8</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>R5F10PLHCLFB#15</t>
+          <t>F1130EVBI</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>UPD703014BYGC-8EU-A</t>
+          <t>F1130NBGI</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>R5F1016AASM#50</t>
+          <t>F1130NBGI8</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>R5F523E6AGFL#30</t>
+          <t>F1150</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>R7F100GMH2DFB#AA0</t>
+          <t>F1150EVBI</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>R5F10EGDANA#U0</t>
+          <t>F1150NBGI</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>R5F103A9ASP#30</t>
+          <t>F1150NBGI8</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>R5F563NFHDFB#10</t>
+          <t>F1152</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>R7FA2E1A92DNH#BA0</t>
+          <t>F1152ANBGI</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>R5F10377DNA#W5</t>
+          <t>F1152ANBGI8</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>R5F101SLAFB#50</t>
+          <t>F1152EVBI</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>R5F104GGGFB#10</t>
+          <t>F1152NBGI</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>R5F100PFAFB#10</t>
+          <t>F1152NBGI8</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>R5F10BGFKNA#G5</t>
+          <t>F1162</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>R5F563TEAGFB#V1</t>
+          <t>F1162AEVBI</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>R5F571MFDDLK#20</t>
+          <t>F1162ANBGI</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>R5F10CLDLFB#H2</t>
+          <t>F1162ANBGI8</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>R5F10AGAKFB#X5</t>
+          <t>F1162BNBGI</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>R8A774E0HA01BN#G0</t>
+          <t>F1162EVBI</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>R5F101FFAFP#V0</t>
+          <t>F1162NBGI</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>R5F10PMJCKFB#15</t>
+          <t>F1162NBGI8</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>R5F10PMEYFB#X5</t>
+          <t>F1178</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>R7FS5D57C3A01CLK#AC1</t>
+          <t>F1178EVBI</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>R5F100GCDFB#30</t>
+          <t>F1178NBGI</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>R5F10PLJYFB#H5</t>
+          <t>F1178NBGI8</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>R5F100MGGFA#V0</t>
+          <t>F1180</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>R5F104LCDFA#X0</t>
+          <t>F1180ENG1NBGI</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>R5F56604DGFN#30</t>
+          <t>F1180ENG1NBGI8</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>R7FA2E2A53CNJ#BA1</t>
+          <t>F1180EVBI</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>RZ/G2LC</t>
+          <t>F1180NBGI8</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>R5F104PJAFA#X0</t>
+          <t>F1192B</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>R5F571MGCGFC#V0</t>
+          <t>F1192BEVBI</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>R7F7010163AFP</t>
+          <t>F1192BNLGK</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>R7FA2E2A34CNK#HA1</t>
+          <t>F1192BNLGK8</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>R5F140PKGFB#50</t>
+          <t>F1200</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>R7S910028CBG#AC0</t>
+          <t>F1200EVBI</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>R5F571MLCDFB#V0</t>
+          <t>F1200EVS</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>R5F56604GGFB#30</t>
+          <t>F1200NBGI</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>R7F100GLL3CFA#HA0</t>
+          <t>F1240</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>R5F100CGALA#U0</t>
+          <t>F1240EVBI</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>R5F51115ADFM#3A</t>
+          <t>F1240EVS</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>R5F104BFGFP#30</t>
+          <t>F1240NBGI</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>R5F101PJDFB#50</t>
+          <t>F1241</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>R5F563NACDLJ#U0</t>
+          <t>F1241EVBI</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>R5F52107CDFN#10</t>
+          <t>F1241EVS</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>R5F109GACJFB#50</t>
+          <t>F1241NBGI</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>R5F56514EDFB#30</t>
+          <t>F1241NBGI8</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>R5F1017ADNA#U0</t>
+          <t>F1300EVBI</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>R5F104GHDFB#50</t>
+          <t>F1300NBGI</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>R7FA4M3AE3CBM#BC0</t>
+          <t>F1300NBGI8</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>R5F100EEANA#20</t>
+          <t>F1320</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>R5F11TLEDFB#55</t>
+          <t>F1320EVBI</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>R5F56514FDLK#20</t>
+          <t>F1320NBGI</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>R5F100MGAFA#30</t>
+          <t>F1320NBGI8</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>R5F10BLECLFB#55</t>
+          <t>F1350</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>R5F52103BGFL#30</t>
+          <t>F1350EVBI</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>R5F100GGGFB#X0</t>
+          <t>F1350NBGI</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>R5F572TKCGFB#10</t>
+          <t>F1350NBGI8</t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>R5F51406ADNE#30</t>
+          <t>F1358</t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>R5F100ADGSP#10</t>
+          <t>F1358EVBI</t>
         </is>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>R5F572NDDDFC#30</t>
+          <t>F1358NBGI</t>
         </is>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>R5F104PGAFB#10</t>
+          <t>F1358NBGI8</t>
         </is>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>R5F5210ABDLK#U0</t>
+          <t>F1370</t>
         </is>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>R5F104FJAFP#10</t>
+          <t>F1370EVBI</t>
         </is>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>R5F100GHDFB#30</t>
+          <t>F1370NBGI</t>
         </is>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>R5F102AADSP#50</t>
+          <t>F1370NBGI8</t>
         </is>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>R5F100FDGFP#10</t>
+          <t>F1375</t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>R5F100GGDNA#U0</t>
+          <t>F1375NBGI</t>
         </is>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>R5F100FCGFP#30</t>
+          <t>F1375NBGI8</t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>R5F104LGGFP#50</t>
+          <t>F1385EVBI</t>
         </is>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>R7S910036CBG#AC0</t>
+          <t>F1385NBGI</t>
         </is>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>R5F571MLGDFB#V0</t>
+          <t>F1385NBGI8</t>
         </is>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>R5F100FJDFP#X0</t>
+          <t>F1420EVBI</t>
         </is>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>R5F10RJ8GFA#10</t>
+          <t>F1420NLGI</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
1. 加入b2b, tender, chrome_IC_search
</commit_message>
<xml_diff>
--- a/TDigikey_upload.xlsx
+++ b/TDigikey_upload.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A500"/>
+  <dimension ref="A1:A508"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -430,3500 +430,3556 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>DA9063L-XXHO1-AT</t>
+          <t>V72C28C150BL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DA9063L-XXHO2</t>
+          <t>V72C36C150BL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DA9063L-XXHO2-AT</t>
+          <t>V72C48C150BL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DA9063-XXHK1-A</t>
+          <t>V72C5C100BL</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DA9063-XXHO1</t>
+          <t>V72C8C100BL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DA9063-XXHO1-A</t>
+          <t>VE-A11-EU</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DA9063-XXHO1-AT</t>
+          <t>VE-A11-IU</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DA9063-XXHO2</t>
+          <t>VE-A11-MU</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DA9063-XXHO2-A</t>
+          <t>VE-A66-CQ</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DA9063-XXHO2-AT</t>
+          <t>VE-AIM-C1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DA9066</t>
+          <t>VE-AIM-E1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DA9066-03</t>
+          <t>VE-AIM-I1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DA9066-EVAL</t>
+          <t>VE-AIM-M1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DA9068</t>
+          <t>VE-ANN-CQ</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DA9068-ABUT2</t>
+          <t>VE-AWW-CU</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DA9070-00V32</t>
+          <t>VE-AWW-IU</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DA9070-00XX</t>
+          <t>VE-AWW-MU</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DA9070-08V32</t>
+          <t>VE-BAMD-CL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DA9070-08V36</t>
+          <t>VE-BAMD-EL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DA9070-09V32</t>
+          <t>VE-BAMD-IL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DA9070-09V36</t>
+          <t>VE-HAM-CL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DA9070-0EV36</t>
+          <t>VE-HAMD-CL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DA9070-FG-EVAL3</t>
+          <t>VE-HAMD-EL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DA9070-ODV32</t>
+          <t>VE-HAMD-IL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DA9070-XXXX</t>
+          <t>VE-HAMD-ML</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>DA9072-80V32</t>
+          <t>VE-HAM-EL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DA9072-82V32</t>
+          <t>VE-HAM-IL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DA9073-00XX</t>
+          <t>VE-HAM-ML</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DA9073-61V32</t>
+          <t>VI-200-CX</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>DA9073-62V32</t>
+          <t>VI-201-CX</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>DA9073-62V36</t>
+          <t>VI-202-CX</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>DA9073-6BV32</t>
+          <t>VI-203-CX</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>DA9073-XXXX</t>
+          <t>VI-204-CX</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>DA9080</t>
+          <t>VI-20B-CX</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>DA9080-XXFC2</t>
+          <t>VI-20F-CX</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>DA9083-XXUUA2</t>
+          <t>VI-20H-CX</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>DA9083-XXUUA6</t>
+          <t>VI-20J-CX</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DA9121-A0V72</t>
+          <t>VI-20K-CX</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>DA9121-A2V72</t>
+          <t>VI-20L-CX</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>DA9121-B0V72</t>
+          <t>VI-20M-CX</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>DA9122-E1V72</t>
+          <t>VI-20N-CX</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DA9122-E1V76</t>
+          <t>VI-20P-CX</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>DA9130-A</t>
+          <t>VI-20R-CX</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>DA9130-XXRT1</t>
+          <t>VI-20T-CX</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>DA9130-XXRT1-A</t>
+          <t>VI-20V-CX</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>DA9130-XXRT2</t>
+          <t>VI-20Y-CX</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>DA9130-XXRT2-A</t>
+          <t>VI-20Z-CX</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DA9130-XXRT2-AT</t>
+          <t>VI-210-CU</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DA9131-A</t>
+          <t>VI-211-CU</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DA9131-XXRT1</t>
+          <t>VI-212-CU</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DA9131-XXRT1-AT</t>
+          <t>VI-213-CU</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>DA9131-XXRT2</t>
+          <t>VI-214-CU</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>DA9131-XXRT2-A</t>
+          <t>VI-21B-CU</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>DA9131-XXRT2-AT</t>
+          <t>VI-21D-CU</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>DA9132-A</t>
+          <t>VI-21F-CU</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>DA9132-XXRT1</t>
+          <t>VI-21J-CU</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>DA9132-XXRT1-AT</t>
+          <t>VI-21L-CU</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>DA9132-XXRT2</t>
+          <t>VI-21M-CU</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DA9132-XXRT2-A</t>
+          <t>VI-21P-CU</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>DA9155M-02U72</t>
+          <t>VI-21R-CV</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>DA9155M-EVAL1</t>
+          <t>VI-21T-CV</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>DA9155M-XXU72</t>
+          <t>VI-21Y-CU</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>DA9168</t>
+          <t>VI-21Z-CU</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>DA9168-XXU72</t>
+          <t>VI-220-CW</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>DA9210-A</t>
+          <t>VI-221-CW</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>DA9211</t>
+          <t>VI-222-CW</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>DA9211-00UU6</t>
+          <t>VI-223-CW</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>DA9211-50UU2</t>
+          <t>VI-224-CW</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>DA9212-00UU2</t>
+          <t>VI-22J-CW</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>DA9212-00UU6</t>
+          <t>VI-22L-CW</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>DA9212-50UU2</t>
+          <t>VI-22M-CW</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>DA9212-AKUU2</t>
+          <t>VI-22N-CW</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DA9213-00UP2</t>
+          <t>VI-22P-CW</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>DA9213-00UP6</t>
+          <t>VI-22R-CW</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>DA9213-50UP2</t>
+          <t>VI-22T-CW</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>DA9213-A-EVAL1</t>
+          <t>VI-22Y-CV</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>DA9213-C1FS2-A</t>
+          <t>VI-230-CU</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>DA9213-C1FS2BB-A</t>
+          <t>VI-231-CU</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>DA9213-EVAL1</t>
+          <t>VI-232-CU</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>DA9213-XXFS1-A</t>
+          <t>VI-233-CU</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>DA9213-XXFSC</t>
+          <t>VI-234-CU</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>DA9213-XXUP2</t>
+          <t>VI-23F-CU</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>DA9214-00FS1-A</t>
+          <t>VI-23H-CU</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>DA9214-00FS2-A</t>
+          <t>VI-23J-CU</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>DA9214-00UP2</t>
+          <t>VI-23L-CU</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>DA9214-50UP2</t>
+          <t>VI-23M-CU</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>DA9214-A</t>
+          <t>VI-23N-CU</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>DA9214-C3FS2-A</t>
+          <t>VI-23P-CU</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>DA9214-XXFSC</t>
+          <t>VI-23V-CU</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>DA9214-XXFSC-AT</t>
+          <t>VI-23Y-CU</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>DA9214-XXUP2</t>
+          <t>VI-23Z-CU</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>DA9215-00UP2</t>
+          <t>VI-240-CU</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>DA9215-00UP6</t>
+          <t>VI-241-CU</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>DA9215-50UP2</t>
+          <t>VI-242-CU</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>DA9215-XXFS1-AT</t>
+          <t>VI-243-CU</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>DA9215-XXFSC</t>
+          <t>VI-244-CU</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>DA9215-XXFSC-A</t>
+          <t>VI-24B-CU</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>DA9215-XXUP2</t>
+          <t>VI-24F-CU</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>DA9215-XXUP6</t>
+          <t>VI-24H-CU</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>DA9217-20V72</t>
+          <t>VI-24J-CU</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>DA9217-20V76</t>
+          <t>VI-24L-CU</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>DA9217-EVAL1</t>
+          <t>VI-24M-CU</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>DA9217-XXV72</t>
+          <t>VI-24N-CU</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>DA9217-XXV76</t>
+          <t>VI-24P-CU</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>DA9220-70V72</t>
+          <t>VI-24V-CU</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>DA9220-70V76</t>
+          <t>VI-24W-CU</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>DA9220-71V72</t>
+          <t>VI-24X-CU</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>DA9220-71V76</t>
+          <t>VI-251-CU</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>DA9220-EVAL1</t>
+          <t>VI-252-CU</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>DA9220-XXV72</t>
+          <t>VI-253-CU</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>DA9224-A</t>
+          <t>VI-254-CU</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>DA9230-00VZ2</t>
+          <t>VI-25B-CU</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>DA9230-07VZ2</t>
+          <t>VI-25F-CU</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>DA9230-09VZ2</t>
+          <t>VI-25H-CU</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>DA9230-0AVZ2</t>
+          <t>VI-25J-CU</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>DA9230-XXVZ2</t>
+          <t>VI-25K-CU</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>DA9231-00VZ2</t>
+          <t>VI-25L-CU</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>DA9231-0BVZ2</t>
+          <t>VI-25N-CU</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>DA9231-0CVZ2</t>
+          <t>VI-25P-CU</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>DA9231-0DVZ2</t>
+          <t>VI-25R-CV</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>DA9231-XXVZ2</t>
+          <t>VI-25T-CV</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>DA9232-81VZ2</t>
+          <t>VI-25V-CV</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>DA9232-82VZ2</t>
+          <t>VI-25W-CV</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>DA9232-XXVZ2</t>
+          <t>VI-25X-CV</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>DA9233-A1VZ2</t>
+          <t>VI-25Y-CU</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>DA9233-XXVZ2</t>
+          <t>VI-25Z-CU</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>DA9313-02VK2</t>
+          <t>VI-260-CU</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>DA9313-02VK6</t>
+          <t>VI-261-CU</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>DA9313-03VK2</t>
+          <t>VI-262-CU</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>DA9313-03VK6</t>
+          <t>VI-263-CU</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>DA9313-04VK2</t>
+          <t>VI-264-CU</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>DA9313-04VK6</t>
+          <t>VI-26B-CU</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>DA9313-08VK2</t>
+          <t>VI-26D-CU</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>DA9313-10VK2</t>
+          <t>VI-26F-CU</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>DA9313-24VK2</t>
+          <t>VI-26H-CU</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>DA9318L</t>
+          <t>VI-26J-CU</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>DA9318L-06UF2</t>
+          <t>VI-26K-CU</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>DA9318M-06UF2</t>
+          <t>VI-26L-CU</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>DG403DVZ</t>
+          <t>VI-26M-CU</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>DG403DY</t>
+          <t>VI-26N-CU</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>DG403DYZ</t>
+          <t>VI-26P-CU</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>DG403EJ</t>
+          <t>VI-26R-CV</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>DG403EY</t>
+          <t>VI-26T-CV</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>DG406DJ</t>
+          <t>VI-26V-CU</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>DG406DJZ</t>
+          <t>VI-26W-CU</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>DG406DY</t>
+          <t>VI-26X-CU</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>DG406DYZ</t>
+          <t>VI-26Y-CU</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>DG406DYZ-T</t>
+          <t>VI-26Z-CU</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>DG406EY</t>
+          <t>VI-270-CY</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>DG407DJ</t>
+          <t>VI-271-CW</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>DG407DJZ</t>
+          <t>VI-272-CW</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>DG407DYZ</t>
+          <t>VI-273-CW</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>DG407DYZ-T</t>
+          <t>VI-274-CW</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>DG407EJ</t>
+          <t>VI-27H-CW</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>DG408DJ</t>
+          <t>VI-27J-CW</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>DG408DJZ</t>
+          <t>VI-27L-CW</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>DG408DVZ</t>
+          <t>VI-27N-CW</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>DG408DYZ</t>
+          <t>VI-27P-CW</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>DG408DYZ-T</t>
+          <t>VI-27R-CW</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>DG409DJ</t>
+          <t>VI-27T-CW</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>DG409DJZ</t>
+          <t>VI-27X-CY</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>DG409DVZ</t>
+          <t>VI-27Y-CW</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>DG409DVZ-T</t>
+          <t>VI-2N0-CU</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>DG409DYZ</t>
+          <t>VI-2N1-CU</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>DG409DYZ-T</t>
+          <t>VI-2N2-CU</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>DG409EJ</t>
+          <t>VI-2N3-CU</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>DG411DVZ-T</t>
+          <t>VI-2N4-CU</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>DG411DYZ</t>
+          <t>VI-2NB-CU</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>DG411DYZ-T</t>
+          <t>VI-2ND-CU</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>DG412DVZ-T</t>
+          <t>VI-2NF-CU</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>DG412DYZ</t>
+          <t>VI-2NH-CU</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>DG412DYZ-T</t>
+          <t>VI-2NJ-CU</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>DG413DJZ</t>
+          <t>VI-2NK-CU</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>DG413DYZ</t>
+          <t>VI-2NL-CU</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>DG413DYZ-T</t>
+          <t>VI-2NM-CU</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>DG441AK/883</t>
+          <t>VI-2NP-CU</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>DG441DJZ</t>
+          <t>VI-2NR-CU</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>DG441DVZ</t>
+          <t>VI-2NT-CU</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>DG441DVZ-T</t>
+          <t>VI-2NV-CU</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>DG441DYZ</t>
+          <t>VI-2NW-CU</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>DG441DYZ-T</t>
+          <t>VI-2NY-CU</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>DG441EY</t>
+          <t>VI-2NZ-CV</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>DG442DJZ</t>
+          <t>VI-2T0-CV</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>DG442DVZ</t>
+          <t>VI-2T1-CV</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>DG442DVZ-T</t>
+          <t>VI-2T2-CV</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>DG442DYZ</t>
+          <t>VI-2T3-CV</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>DG442DYZ-T</t>
+          <t>VI-2T4-CV</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>DG444DVZ-T</t>
+          <t>VI-2TF-CV</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>DG444DY</t>
+          <t>VI-2TJ-CV</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>DG444DYZ</t>
+          <t>VI-2TL-CV</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>DG444DYZ-T</t>
+          <t>VI-2TP-CV</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>DG445DJ</t>
+          <t>VI-2TY-CV</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>DG445DVZ</t>
+          <t>VI-2V0-CY</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>DG445DVZ-T</t>
+          <t>VI-2V1-CX</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>DG445DY</t>
+          <t>VI-2V2-CX</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>DG445DYZ</t>
+          <t>VI-2V3-CX</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>DG445DYZ-T</t>
+          <t>VI-2V4-CX</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>EL4340IU</t>
+          <t>VI-2VJ-CX</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>EL4340IU-T13</t>
+          <t>VI-2VK-CX</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>EL4340IU-T7</t>
+          <t>VI-2VL-CX</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>EL4340IUZ</t>
+          <t>VI-2VM-CX</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>EL4340IUZ-T13</t>
+          <t>VI-2VN-CX</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>EL4340IUZ-T7</t>
+          <t>VI-2VP-CX</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>EL4543IL</t>
+          <t>VI-2VR-CX</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>EL4543IL-T13</t>
+          <t>VI-2VT-CY</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>EL4543ILZ-T7</t>
+          <t>VI-2VV-CY</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>EL4543IU</t>
+          <t>VI-2VY-CX</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>EL4543IUZ-T7</t>
+          <t>VI-2W0-CV</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>EL5106IS</t>
+          <t>VI-2W1-CV</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>EL5106ISZ</t>
+          <t>VI-2W2-CV</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>EL5106ISZ-T13</t>
+          <t>VI-2W3-CV</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>EL5106IWZ-T7</t>
+          <t>VI-2W4-CV</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>EL5106IWZ-T7A</t>
+          <t>VI-2WB-CV</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>EL5111IWTZ-T7</t>
+          <t>VI-2WD-CV</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>EL5111IWTZ-T7A</t>
+          <t>VI-2WF-CV</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>EL5111IYEZ</t>
+          <t>VI-2WH-CV</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>EL5111IYEZ-T13</t>
+          <t>VI-2WJ-CV</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>EL5111IYEZ-T7</t>
+          <t>VI-2WK-CV</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>EL5111TIWTZ-T7</t>
+          <t>VI-2WL-CV</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>EL5111TIWTZ-T7A</t>
+          <t>VI-2WM-CV</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>EL5160ISZ</t>
+          <t>VI-2WN-CV</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>EL5160ISZ-T7A</t>
+          <t>VI-2WP-CV</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>EL5160IWZ-T7</t>
+          <t>VI-2WR-CW</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>EL5160IWZ-T7A</t>
+          <t>VI-2WT-CW</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>EL5161IC-T7A</t>
+          <t>VI-2WW-CV</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>EL5161IWZ-T7</t>
+          <t>VI-2WY-CV</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>EL5161IWZ-T7A</t>
+          <t>VI-2WZ-CV</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>EL5166ISZ</t>
+          <t>VI-A11-CU</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>EL5166ISZ-T7</t>
+          <t>VI-A11-IU</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>EL5166IWZ-T7</t>
+          <t>VI-A11-MU</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>EL5166IWZ-T7A</t>
+          <t>VI-A33-CQ</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>EL5172IS</t>
+          <t>VI-A33-IQ</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>EL5172ISZ</t>
+          <t>VI-A66-CQ</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>EL5172ISZ-T7</t>
+          <t>VI-A66-EQ</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>EL5172ISZ-T7A</t>
+          <t>VI-A66-IQ</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>EL5172IY-T7</t>
+          <t>VI-A66-MQ</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>EL5172IYZ-T13</t>
+          <t>VI-AIM-C1</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>EL5172IYZ-T7</t>
+          <t>VI-AIM-E1</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>EL5220CY</t>
+          <t>VI-AIM-I1</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>EL5220CY-T13</t>
+          <t>VI-AIM-M1</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>EL5220CY-T7</t>
+          <t>VI-ANN-CQ</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>EL5220CYZ</t>
+          <t>VI-ANN-IQ</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>EL5220CYZ-T13</t>
+          <t>VI-ARMB-C21</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>EL5220CYZ-T7</t>
+          <t>VI-ARMB-C22</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>EL5220TILZ-T13</t>
+          <t>VI-ARMB-C222</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>EL5220TIYZ</t>
+          <t>VI-ARMB-C223</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>EL5220TIYZ-T13</t>
+          <t>VI-ARMB-C2G</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>EL5220TIYZ-T7</t>
+          <t>VI-ARMB-C2N</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>EL5262IY-T7</t>
+          <t>VI-ARMB-E21</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>EL5262IYZ</t>
+          <t>VI-ARMB-E22</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>EL5262IYZ-T13</t>
+          <t>VI-ARMB-H21</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>EL5262IYZ-T7</t>
+          <t>VI-ARMB-H22</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>EL5263IS-T13</t>
+          <t>VI-ARMB-H2G</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>EL5263IS-T7</t>
+          <t>VI-ARMB-H2G3</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>EL5263ISZ</t>
+          <t>VI-ARMB-H2N</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>EL5263ISZ-T13</t>
+          <t>VI-ARMB-H2N2</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>EL5263ISZ-T7</t>
+          <t>VI-ARMB-T21</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>EL5263IYZ</t>
+          <t>VI-ARMB-T22</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>EL5263IYZ-T13</t>
+          <t>VI-ARMB-T222</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>EL5306IS</t>
+          <t>VI-ARMB-T223</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>EL5306IS-T13</t>
+          <t>VI-ARMB-T2G</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>EL5306ISZ-T7</t>
+          <t>VI-ARMB-T2N</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>EL5306IU-T13</t>
+          <t>VI-ARMB-T2S</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>EL5306IUZ</t>
+          <t>VI-ARM-C11</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>EL5306IUZ-T13</t>
+          <t>VI-ARM-C12</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>EL5306IUZ-T7</t>
+          <t>VI-ARM-C122</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>EL5375IU</t>
+          <t>VI-ARM-C123</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>EL5375IU-T13</t>
+          <t>VI-ARM-C1F</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>EL5375IU-T7</t>
+          <t>VI-ARM-C1F3</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>EL5375IUZ-T7</t>
+          <t>VI-ARM-C1G</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>EL5378IU</t>
+          <t>VI-ARM-E12</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>EL5378IU-T7</t>
+          <t>VI-ARM-E1G</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>EL5378IUZ</t>
+          <t>VI-ARM-H12</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>EL5378IUZ-T13</t>
+          <t>VI-ARM-H122</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>EL5378IUZ-T7</t>
+          <t>VI-ARM-H123</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>EL5420CR</t>
+          <t>VI-ARM-H1N</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>EL5420CR-T13</t>
+          <t>VI-ARM-T11</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>EL5420CR-T7</t>
+          <t>VI-ARM-T12</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>EL5420CRZ</t>
+          <t>VI-ARM-T122</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>EL5420CRZ-T13</t>
+          <t>VI-ARM-T123</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>EL5420CRZ-T7</t>
+          <t>VI-ARM-T1G</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>EL5420CRZ-T7A</t>
+          <t>VI-ARM-T1N</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>EL5420CSZ</t>
+          <t>VI-ARM-T1N3</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>EL5420TILZ</t>
+          <t>VI-ARM-T1S</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>EL5420TIRZ</t>
+          <t>VI-AWW-CU</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>EL5420TISZ-T13</t>
+          <t>VI-AWW-EU</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>EL5462IS</t>
+          <t>VI-AWW-IU</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>EL5462IS-T13</t>
+          <t>VI-AWW-MU</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>EL5462IS-T7</t>
+          <t>VI-BAMD-CL</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>EL5462ISZ</t>
+          <t>VI-BAMD-EL</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>EL5462ISZ-T13</t>
+          <t>VI-BAMD-IL</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>EL5462ISZ-T7</t>
+          <t>VI-BAMD-ML</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>EL7104CN</t>
+          <t>VI-HAM-CL</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>EL7104CNZ</t>
+          <t>VI-HAMD-CL</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>EL7104CS</t>
+          <t>VI-HAMD-EL</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>EL7104CSZ</t>
+          <t>VI-HAMD-IL</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>EL7104CSZ-T13</t>
+          <t>VI-HAMD-ML</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>EL7104CSZ-T7</t>
+          <t>VI-HAM-EL</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>EL7202CN</t>
+          <t>VI-HAM-IL</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>EL7202CS</t>
+          <t>VI-HAM-ML</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>EL7202CS-T7</t>
+          <t>VI-J00-CY</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>EL7202CSZ</t>
+          <t>VI-J01-CX</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>EL7202CSZ-T7</t>
+          <t>VI-J02-CX</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>EL7212CN</t>
+          <t>VI-J03-CX</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>EL7212CNZ</t>
+          <t>VI-J04-CX</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>EL7212CS</t>
+          <t>VI-J0B-CX</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>EL7212CSZ</t>
+          <t>VI-J0F-CX</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>EL7212CSZ-T13</t>
+          <t>VI-J0J-CX</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>EL7212CSZ-T7</t>
+          <t>VI-J0K-CX</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>EL7222CS</t>
+          <t>VI-J0L-CX</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>EL7222CSE9044-T7</t>
+          <t>VI-J0M-CX</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>EL7222CS-T7</t>
+          <t>VI-J0N-CX</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>EL7222CSZ</t>
+          <t>VI-J0P-CX</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>EL7222CSZ-T13</t>
+          <t>VI-J0R-CY</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>EL7222CSZ-T7</t>
+          <t>VI-J0T-CY</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>EL7232CNZ</t>
+          <t>VI-J0V-CY</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>EL7232CS</t>
+          <t>VI-J0X-CY</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>EL7232CSZ</t>
+          <t>VI-J0Y-CX</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>EL7232CSZ-T13</t>
+          <t>VI-J0Z-CX</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>EL7242CS</t>
+          <t>VI-J11-CW</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>EL7242CS-T13</t>
+          <t>VI-J12-CW</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>EL7242CS-T7</t>
+          <t>VI-J13-CW</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>EL7242CSZ-T13</t>
+          <t>VI-J14-CW</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>EL7242CSZ-T7</t>
+          <t>VI-J1B-CW</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>EL7252CN</t>
+          <t>VI-J1F-CW</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>EL7252CSZ</t>
+          <t>VI-J1H-CW</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>EL7252CSZ-T13</t>
+          <t>VI-J1J-CW</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>EL7252CSZ-T7</t>
+          <t>VI-J1L-CW</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>EL7530IY</t>
+          <t>VI-J1M-CW</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>EL7530IY-T13</t>
+          <t>VI-J1P-CW</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>EL7530IY-T7</t>
+          <t>VI-J1R-CX</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>EL7530IYZ-T13</t>
+          <t>VI-J1T-CX</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>EL7530IYZ-T13S2695</t>
+          <t>VI-J1V-CW</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>EL7530IYZ-T7</t>
+          <t>VI-J1Y-CW</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>EL7531EVAL1Z</t>
+          <t>VI-J1Z-CW</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>EL7531IY</t>
+          <t>VI-J20-CY</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>EL7531IY-T7</t>
+          <t>VI-J21-CW</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>EL7531IYZ</t>
+          <t>VI-J2V-CY</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>EL7531IYZ-T13</t>
+          <t>VI-J2W-CY</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>EL7531IYZ-T7</t>
+          <t>VI-J2Y-CY</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>EL7536EVAL1</t>
+          <t>VI-J2Z-CY</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>EL7536IY</t>
+          <t>VI-J31-CW</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>EL7536IY-T7</t>
+          <t>VI-J32-CW</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>EL7536IYZ</t>
+          <t>VI-J33-CW</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>EL7536IYZ-T</t>
+          <t>VI-J34-CW</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>EL7536IYZ-T13</t>
+          <t>VI-J3F-CW</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>EL7536IYZ-T7</t>
+          <t>VI-J3H-CW</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>EL8201IS</t>
+          <t>VI-J3L-CW</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>EL8201IS-T13</t>
+          <t>VI-J3M-CW</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>EL8201IS-T7</t>
+          <t>VI-J3T-CX</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>EL8201ISZ</t>
+          <t>VI-J3V-CW</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>EL8201ISZ-T13</t>
+          <t>VI-J3Y-CW</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>EL8201ISZ-T7</t>
+          <t>VI-J3Z-CW</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>EXP8602-DNT</t>
+          <t>VI-J41-CW</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>F0109</t>
+          <t>VI-J42-CW</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>F0109EVB</t>
+          <t>VI-J43-CW</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>F0109NBTI</t>
+          <t>VI-J44-CW</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>F0109NBTI8</t>
+          <t>VI-J4J-CW</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>F0110EVB</t>
+          <t>VI-J4K-CW</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>F0110NBTI</t>
+          <t>VI-J4L-CW</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>F0110NBTI8</t>
+          <t>VI-J50-CW</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>F0111EVB</t>
+          <t>VI-J51-CW</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>F0111EVB-2P6</t>
+          <t>VI-J52-CW</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>F0111NBTI</t>
+          <t>VI-J53-CW</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>F0111NBTI8</t>
+          <t>VI-J54-CW</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>F0424EVBK</t>
+          <t>VI-J5B-CW</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>F0424NTGK</t>
+          <t>VI-J5D-CW</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>F0424NTGK8</t>
+          <t>VI-J5F-CW</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>F0440EVBI</t>
+          <t>VI-J5H-CW</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>F0440NBGI</t>
+          <t>VI-J5J-CW</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>F0440NBGI/W</t>
+          <t>VI-J5L-CW</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>F0440NBGI8</t>
+          <t>VI-J5M-CW</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>F0443EVB</t>
+          <t>VI-J5N-CW</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>F0443LGRI8</t>
+          <t>VI-J5R-CX</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>F0448EVB</t>
+          <t>VI-J5T-CX</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>F0448EVS</t>
+          <t>VI-J5Y-CW</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>F0448NBGK</t>
+          <t>VI-J60-CW</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>F0448NBGK8</t>
+          <t>VI-J61-CW</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>F0452BEVB</t>
+          <t>VI-J62-CW</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>F0452BLEGK</t>
+          <t>VI-J63-CW</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>F0452BLEGK8</t>
+          <t>VI-J64-CW</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>F0452CEVB</t>
+          <t>VI-J6B-CW</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>F0452CLFGK</t>
+          <t>VI-J6D-CW</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>F0452CLFGK8</t>
+          <t>VI-J6F-CW</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>F0453B</t>
+          <t>VI-J6H-CW</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>F0453BEVB</t>
+          <t>VI-J6J-CW</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>F0453BLEGK</t>
+          <t>VI-J6K-CW</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>F0453BLEGK8</t>
+          <t>VI-J6L-CW</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>F0453CEVB</t>
+          <t>VI-J6M-CW</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>F0453CLEGK</t>
+          <t>VI-J6N-CW</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>F0453CLFGK</t>
+          <t>VI-J6P-CW</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>F0453CLFGK8</t>
+          <t>VI-J6R-CX</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>F0480EVB-HBI</t>
+          <t>VI-J6T-CX</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>F0480EVBI</t>
+          <t>VI-J6X-CW</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>F0480EVB-LBI</t>
+          <t>VI-J6Y-CW</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>F0480EVB-MBI</t>
+          <t>VI-J6Z-CW</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>F0480EVS-HBI</t>
+          <t>VI-J70-CY</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>F0480EVS-LBI</t>
+          <t>VI-J71-CX</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>F0480EVS-MBI</t>
+          <t>VI-J72-CX</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>F0480NBGI</t>
+          <t>VI-J73-CX</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>F0502EVBI</t>
+          <t>VI-J74-CX</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>F0502NLGI</t>
+          <t>VI-J7J-CX</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>F0502NLGI8</t>
+          <t>VI-J7L-CX</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>F0552EVBI</t>
+          <t>VI-J7M-CX</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>F0552NLGI8</t>
+          <t>VI-J7P-CX</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>F0562EVBI</t>
+          <t>VI-J7R-CY</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>F0562NLGI</t>
+          <t>VI-J7W-CY</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>F0562NLGI8</t>
+          <t>VI-J7X-CY</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>F1100</t>
+          <t>VI-J7Y-CY</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>F1100ANBGI</t>
+          <t>VI-J7Z-CY</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>F1100BNBGI</t>
+          <t>VI-JN0-CX</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>F1100BNBGI8</t>
+          <t>VI-JN1-CW</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>F1100NBGI</t>
+          <t>VI-JN2-CW</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>F1100NBGI8</t>
+          <t>VI-JN3-CW</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>F1102</t>
+          <t>VI-JN4-CW</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>F1102EVBI</t>
+          <t>VI-JNB-CW</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>F1102NBGI8</t>
+          <t>VI-JND-CW</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>F1102NBGI8(4)</t>
+          <t>VI-JNF-CW</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>F1129EVB</t>
+          <t>VI-JNJ-CW</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>F1129HBNELI</t>
+          <t>VI-JNL-CW</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>F1129HBNELI8</t>
+          <t>VI-JNM-CW</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>F1129LBNELI8</t>
+          <t>VI-JNN-CW</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>F1129MB</t>
+          <t>VI-JNR-CX</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>F1129MBEVB</t>
+          <t>VI-JNW-CX</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>F1129MBNELI</t>
+          <t>VI-JNX-CX</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>F1129MBNELI8</t>
+          <t>VI-JNY-CW</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>F1130EVBI</t>
+          <t>VI-JNZ-CW</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>F1130NBGI</t>
+          <t>VI-JT0-CX</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>F1130NBGI8</t>
+          <t>VI-JT1-CW</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>F1150</t>
+          <t>VI-JT2-CW</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>F1150EVBI</t>
+          <t>VI-JT3-CW</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>F1150NBGI</t>
+          <t>VI-JT4-CW</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>F1150NBGI8</t>
+          <t>VI-JTF-CW</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>F1152</t>
+          <t>VI-JTJ-CW</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>F1152ANBGI</t>
+          <t>VI-JTL-CW</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>F1152ANBGI8</t>
+          <t>VI-JTM-CW</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>F1152EVBI</t>
+          <t>VI-JTP-CW</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>F1152NBGI</t>
+          <t>VI-JTR-CX</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>F1152NBGI8</t>
+          <t>VI-JTT-CX</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>F1162</t>
+          <t>VI-JTX-CX</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>F1162AEVBI</t>
+          <t>VI-JTY-CW</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>F1162ANBGI</t>
+          <t>VI-JV0-CY</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>F1162ANBGI8</t>
+          <t>VI-JV1-CY</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>F1162BNBGI</t>
+          <t>VI-JV2-CY</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>F1162EVBI</t>
+          <t>VI-JV3-CY</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>F1162NBGI</t>
+          <t>VI-JV4-CY</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>F1162NBGI8</t>
+          <t>VI-JVJ-CY</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>F1178</t>
+          <t>VI-JVK-CY</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>F1178EVBI</t>
+          <t>VI-JVL-CY</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>F1178NBGI</t>
+          <t>VI-JVM-CY</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>F1178NBGI8</t>
+          <t>VI-JVN-CY</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>F1180</t>
+          <t>VI-JVP-CY</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>F1180ENG1NBGI</t>
+          <t>VI-JVR-CY</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>F1180ENG1NBGI8</t>
+          <t>VI-JVT-CY</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>F1180EVBI</t>
+          <t>VI-JVV-CY</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>F1180NBGI8</t>
+          <t>VI-JVY-CY</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>F1192B</t>
+          <t>VI-JW0-CW</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>F1192BEVBI</t>
+          <t>VI-JW1-CW</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>F1192BNLGK</t>
+          <t>VI-JW2-CW</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>F1192BNLGK8</t>
+          <t>VI-JW3-CW</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>F1200</t>
+          <t>VI-JW4-CW</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>F1200EVBI</t>
+          <t>VI-JWB-CW</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>F1200EVS</t>
+          <t>VI-JWD-CW</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>F1200NBGI</t>
+          <t>VI-JWF-CW</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>F1240</t>
+          <t>VI-JWJ-CW</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>F1240EVBI</t>
+          <t>VI-JWK-CW</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>F1240EVS</t>
+          <t>VI-JWL-CW</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>F1240NBGI</t>
+          <t>VI-JWM-CW</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>F1241</t>
+          <t>VI-JWN-CW</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>F1241EVBI</t>
+          <t>VI-JWP-CW</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>F1241EVS</t>
+          <t>VI-JWR-CX</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>F1241NBGI</t>
+          <t>VI-JWT-CX</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>F1241NBGI8</t>
+          <t>VI-JWY-CW</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>F1300EVBI</t>
+          <t>VI-JWZ-CW</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>F1300NBGI</t>
+          <t>VIT028H3U600C000</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>F1300NBGI8</t>
+          <t>VIT028H3U600D000</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>F1320</t>
+          <t>VIT028H6U1000C000</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>F1320EVBI</t>
+          <t>VIT270H3U600C002</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>F1320NBGI</t>
+          <t>VTM2308S60Z0825T00</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>F1320NBGI8</t>
+          <t>VTM2308S60Z1513T00</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>F1350</t>
+          <t>VTM48EF012T130C01</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>F1350EVBI</t>
+          <t>VTM48EF040T050B00</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>F1350NBGI</t>
+          <t>VTM48EF040T050B0R</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>F1350NBGI8</t>
+          <t>VTM48EF060T040A00</t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>F1358</t>
+          <t>VTM48EF080T030A00</t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>F1358EVBI</t>
+          <t>VTM48EF096T025A00</t>
         </is>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>F1358NBGI</t>
+          <t>VTM48EF096T025A01</t>
         </is>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>F1358NBGI8</t>
+          <t>VTM48EF096T027A00</t>
         </is>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>F1370</t>
+          <t>VTM48EF120T025A00</t>
         </is>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>F1370EVBI</t>
+          <t>VTM48EF120T025A0R</t>
         </is>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>F1370NBGI</t>
+          <t>VTM48EF160T015A00</t>
         </is>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>F1370NBGI8</t>
+          <t>VTM48EF160T015A01</t>
         </is>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>F1375</t>
+          <t>VTM48EF240T012A00</t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>F1375NBGI</t>
+          <t>VTM48EF240T012A01</t>
         </is>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>F1375NBGI8</t>
+          <t>VTM48EF320T009A00</t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>F1385EVBI</t>
+          <t>VTM48EF320T009A01</t>
         </is>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>F1385NBGI</t>
+          <t>VTM48EF480T006A00</t>
         </is>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>F1385NBGI8</t>
+          <t>VTM48EF480T006A01</t>
         </is>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>F1420EVBI</t>
+          <t>VTM48EH040T025B00</t>
         </is>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>F1420NLGI</t>
+          <t>VTM48EH060T020A00</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>VTM48EH060T020A01</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>VTM48EH120T010B00</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>VTM48EH120T010B01</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>VTM48KP020T088AA1</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>VTM48KP020T095BA0</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>VTM48MP010T107AA1</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>VTM48MP010T135AA0</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>VTM48MP012T130AA0</t>
         </is>
       </c>
     </row>

</xml_diff>